<commit_message>
Ran through latest numbers
Cleaned up the folder as well.
</commit_message>
<xml_diff>
--- a/Team_Results.xlsx
+++ b/Team_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/GitHub/Hattrick_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbrockmann\Documents\GitHub\Hattrick_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D635D83-9CF4-7A44-A38F-41A236D81726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9BE8E3-B216-4C2B-A738-BA49E1993ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19760" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>POS</t>
   </si>
@@ -169,13 +169,10 @@
     <t>IM</t>
   </si>
   <si>
+    <t>LW</t>
+  </si>
+  <si>
     <t>RW</t>
-  </si>
-  <si>
-    <t>RB</t>
-  </si>
-  <si>
-    <t>LW</t>
   </si>
   <si>
     <t>LB</t>
@@ -185,7 +182,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +195,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -208,7 +211,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,8 +254,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,13 +560,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -637,7 +640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -668,11 +671,8 @@
       <c r="X2">
         <v>9.7900000000000009</v>
       </c>
-      <c r="Y2">
-        <v>2.84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -728,10 +728,10 @@
         <v>9.9699999999999989</v>
       </c>
       <c r="Y3">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -769,7 +769,7 @@
         <v>12.18</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -801,7 +801,7 @@
         <v>11.807</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -869,10 +869,10 @@
         <v>9.49</v>
       </c>
       <c r="Y6">
-        <v>3.18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -919,10 +919,10 @@
         <v>9.33</v>
       </c>
       <c r="Y7">
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+        <v>2.57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -993,10 +993,10 @@
         <v>9.0299999999999994</v>
       </c>
       <c r="Y8">
-        <v>4.0599999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1046,10 +1046,10 @@
         <v>8.9</v>
       </c>
       <c r="Y9">
-        <v>2.92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1119,11 +1119,8 @@
       <c r="X10">
         <v>8.32</v>
       </c>
-      <c r="Y10">
-        <v>2.54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1170,10 +1167,10 @@
         <v>12.15</v>
       </c>
       <c r="Y11">
-        <v>3.36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1214,7 +1211,7 @@
         <v>11.85</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1240,7 +1237,7 @@
         <v>10.33</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1269,7 +1266,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1298,7 +1295,7 @@
         <v>10.119999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1327,7 +1324,7 @@
         <v>10.17</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1353,7 +1350,7 @@
         <v>9.4099999999999984</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1390,8 +1387,11 @@
       <c r="W18">
         <v>11.71</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y18">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1423,10 +1423,10 @@
         <v>11.79</v>
       </c>
       <c r="Y19">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1491,8 +1491,11 @@
       <c r="O22">
         <v>8.7100000000000009</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y22">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1503,14 +1506,14 @@
         <v>6.55</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -1525,22 +1528,25 @@
       <c r="H24" t="s">
         <v>27</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J24" t="s">
         <v>48</v>
       </c>
       <c r="K24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L24" t="s">
         <v>43</v>
       </c>
       <c r="M24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N24" t="s">
+        <v>47</v>
+      </c>
+      <c r="O24" t="s">
         <v>48</v>
       </c>
       <c r="P24" t="s">
@@ -1550,16 +1556,16 @@
         <v>48</v>
       </c>
       <c r="R24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T24" t="s">
         <v>43</v>
       </c>
       <c r="U24" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="V24" t="s">
         <v>47</v>
@@ -1567,8 +1573,12 @@
       <c r="W24" t="s">
         <v>47</v>
       </c>
+      <c r="X24" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="138" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>